<commit_message>
Added new metadata columns
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1653D7-4448-42BC-8295-E762896DDC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70A5F3-1A7C-42B8-8905-687E0365FD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Field Name</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>Employee_Survey_Data.csv</t>
+  </si>
+  <si>
+    <t>Background Color</t>
+  </si>
+  <si>
+    <t>#FFFFDD</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Text Align</t>
+  </si>
+  <si>
+    <t>Font Bold</t>
   </si>
 </sst>
 </file>
@@ -457,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A443A47E-CD8A-44BA-8C86-60756BA41290}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -469,9 +484,10 @@
     <col min="2" max="2" width="23.07421875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.3046875" customWidth="1"/>
     <col min="5" max="5" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -490,8 +506,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -507,8 +532,17 @@
       <c r="F2">
         <v>14</v>
       </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -524,8 +558,14 @@
       <c r="E3">
         <v>6</v>
       </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -540,6 +580,12 @@
       </c>
       <c r="E4">
         <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated column width calclation
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F85D9C-233E-4A6E-9AA0-B9C45B2B1370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAD7E0C-8334-4A44-9DDF-534225A2331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>Field Name</t>
   </si>
@@ -530,7 +530,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -633,7 +633,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -656,7 +656,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -726,6 +726,15 @@
       </c>
       <c r="D8">
         <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
       </c>
       <c r="J8" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Changed to XLSX output
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAD7E0C-8334-4A44-9DDF-534225A2331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215B348D-8A70-4D45-8AC5-9D1777E206EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Field Name</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>$#,###</t>
+  </si>
+  <si>
+    <t>Page Orientation</t>
+  </si>
+  <si>
+    <t>Landscape</t>
+  </si>
+  <si>
+    <t>Print Pages Width</t>
   </si>
 </sst>
 </file>
@@ -197,7 +206,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -208,6 +237,48 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0">
+  <autoFilter ref="A1:J8" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{536BAD92-DDD9-4494-936F-87D0426E704B}" name="Report Name"/>
+    <tableColumn id="2" xr3:uid="{6A91D369-F2C3-4116-8219-E95FB21560C7}" name="Field Name" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E70DEC8B-06B4-4D01-BFA5-944FFB97C62F}" name="Is Header"/>
+    <tableColumn id="4" xr3:uid="{1AFD82FA-9A46-434F-AAE3-BF586F79557D}" name="Column Width"/>
+    <tableColumn id="5" xr3:uid="{9A54C87D-A906-4FB0-B37E-487CA6301F8E}" name="Font Size"/>
+    <tableColumn id="6" xr3:uid="{A6A0D0BC-B207-453A-8098-A7CA62B131C1}" name="Background Color"/>
+    <tableColumn id="7" xr3:uid="{9DCBC3B1-B588-4424-98D7-0332156B885E}" name="Text Align"/>
+    <tableColumn id="8" xr3:uid="{51C8C91B-9DE8-47A1-91FA-4305930561A8}" name="Font Bold"/>
+    <tableColumn id="9" xr3:uid="{70D5DE6C-14DB-4298-8D02-0C070ABB7466}" name="Font Name"/>
+    <tableColumn id="10" xr3:uid="{3B76F452-F0AE-4EEE-8206-08977C35E851}" name="Number Format"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}" name="Table2" displayName="Table2" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{819CCBB3-CE38-46C5-BF73-9CAC9404EA8B}" name="Report Name"/>
+    <tableColumn id="2" xr3:uid="{05D5A490-4E2E-476F-BC4B-0E02930681C1}" name="CSV File"/>
+    <tableColumn id="3" xr3:uid="{4ABA2077-D15A-4C80-80AE-C8CA6FF82335}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{032540CA-C8B4-4401-8337-0BA2943F47FD}" name="Font Size"/>
+    <tableColumn id="5" xr3:uid="{FD05CA8E-2FF6-4482-A667-AF6A65E699F6}" name="Font Bold"/>
+    <tableColumn id="6" xr3:uid="{FDC8A75C-3349-4AAA-AF78-CD0E21F747FC}" name="Font Color"/>
+    <tableColumn id="7" xr3:uid="{61C0565E-B0AB-4FA1-B80E-D0BA900ECEF2}" name="Font Name"/>
+    <tableColumn id="8" xr3:uid="{137F01B8-CF74-4619-95FF-80537C14834D}" name="Header Background Color"/>
+    <tableColumn id="9" xr3:uid="{6E25A935-B2DA-4803-BCE0-5704FE01B154}" name="Header Font Color"/>
+    <tableColumn id="10" xr3:uid="{5BE2E524-EFC9-4F41-BE41-FBFB34D249E5}" name="Header Font Size"/>
+    <tableColumn id="11" xr3:uid="{F71558F5-41A4-4F58-A653-BB17CF809C18}" name="Header Font Bold"/>
+    <tableColumn id="12" xr3:uid="{18D32756-3EB2-49B5-8AC4-B585743C00C7}" name="Header Font Name"/>
+    <tableColumn id="13" xr3:uid="{2578C21A-B4B2-498A-A2FF-421E5319AB08}" name="Page Orientation"/>
+    <tableColumn id="14" xr3:uid="{BB9CFB95-A57B-44DD-B45C-3A1BB76A0E70}" name="Print Pages Width"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,16 +600,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A443A47E-CD8A-44BA-8C86-60756BA41290}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.3046875" customWidth="1"/>
-    <col min="4" max="4" width="12.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3828125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="9.921875" customWidth="1"/>
+    <col min="6" max="6" width="16.84375" customWidth="1"/>
+    <col min="7" max="7" width="10.3046875" customWidth="1"/>
+    <col min="8" max="8" width="10.15234375" customWidth="1"/>
+    <col min="9" max="9" width="11.4609375" customWidth="1"/>
+    <col min="10" max="10" width="15.23046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -742,15 +819,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C007B5-97FC-4202-9E75-B2839591FD10}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -758,18 +838,20 @@
     <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.07421875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.07421875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.07421875" customWidth="1"/>
-    <col min="8" max="8" width="21.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.69140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.921875" customWidth="1"/>
+    <col min="5" max="5" width="10.15234375" customWidth="1"/>
+    <col min="6" max="6" width="10.921875" customWidth="1"/>
+    <col min="7" max="7" width="11.4609375" customWidth="1"/>
+    <col min="8" max="8" width="23.15234375" customWidth="1"/>
+    <col min="9" max="9" width="17.23046875" customWidth="1"/>
+    <col min="10" max="10" width="16.23046875" customWidth="1"/>
+    <col min="11" max="11" width="16.4609375" customWidth="1"/>
+    <col min="12" max="12" width="17.765625" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -806,8 +888,14 @@
       <c r="L1" t="s">
         <v>28</v>
       </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -843,10 +931,19 @@
       </c>
       <c r="L2" t="s">
         <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Wrap Text field
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215B348D-8A70-4D45-8AC5-9D1777E206EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A054CC88-7FE6-4D4F-A723-C887249BFA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>Field Name</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Print Pages Width</t>
+  </si>
+  <si>
+    <t>Wrap Text</t>
   </si>
 </sst>
 </file>
@@ -240,9 +243,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0">
-  <autoFilter ref="A1:J8" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0">
+  <autoFilter ref="A1:K8" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{536BAD92-DDD9-4494-936F-87D0426E704B}" name="Report Name"/>
     <tableColumn id="2" xr3:uid="{6A91D369-F2C3-4116-8219-E95FB21560C7}" name="Field Name" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E70DEC8B-06B4-4D01-BFA5-944FFB97C62F}" name="Is Header"/>
@@ -252,6 +255,7 @@
     <tableColumn id="7" xr3:uid="{9DCBC3B1-B588-4424-98D7-0332156B885E}" name="Text Align"/>
     <tableColumn id="8" xr3:uid="{51C8C91B-9DE8-47A1-91FA-4305930561A8}" name="Font Bold"/>
     <tableColumn id="9" xr3:uid="{70D5DE6C-14DB-4298-8D02-0C070ABB7466}" name="Font Name"/>
+    <tableColumn id="11" xr3:uid="{41856FA6-3460-4871-88F9-7A854FBFECD8}" name="Wrap Text"/>
     <tableColumn id="10" xr3:uid="{3B76F452-F0AE-4EEE-8206-08977C35E851}" name="Number Format"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -598,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A443A47E-CD8A-44BA-8C86-60756BA41290}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -614,11 +618,11 @@
     <col min="6" max="6" width="16.84375" customWidth="1"/>
     <col min="7" max="7" width="10.3046875" customWidth="1"/>
     <col min="8" max="8" width="10.15234375" customWidth="1"/>
-    <col min="9" max="9" width="11.4609375" customWidth="1"/>
-    <col min="10" max="10" width="15.23046875" customWidth="1"/>
+    <col min="9" max="10" width="11.4609375" customWidth="1"/>
+    <col min="11" max="11" width="15.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -647,10 +651,13 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -676,7 +683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -699,7 +706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -710,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -721,8 +728,11 @@
       <c r="I4" t="s">
         <v>24</v>
       </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -745,7 +755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -768,7 +778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -791,7 +801,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -813,7 +823,7 @@
       <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -829,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C007B5-97FC-4202-9E75-B2839591FD10}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Added Border Color field
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A054CC88-7FE6-4D4F-A723-C887249BFA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C758EF20-991A-4842-8EA2-737D2C8D8FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Field Name</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Wrap Text</t>
+  </si>
+  <si>
+    <t>Border Color</t>
+  </si>
+  <si>
+    <t>#333333</t>
   </si>
 </sst>
 </file>
@@ -263,9 +269,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}" name="Table2" displayName="Table2" ref="A1:N2" totalsRowShown="0">
-  <autoFilter ref="A1:N2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}" name="Table2" displayName="Table2" ref="A1:O2" totalsRowShown="0">
+  <autoFilter ref="A1:O2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{819CCBB3-CE38-46C5-BF73-9CAC9404EA8B}" name="Report Name"/>
     <tableColumn id="2" xr3:uid="{05D5A490-4E2E-476F-BC4B-0E02930681C1}" name="CSV File"/>
     <tableColumn id="3" xr3:uid="{4ABA2077-D15A-4C80-80AE-C8CA6FF82335}" name="Title"/>
@@ -273,6 +279,7 @@
     <tableColumn id="5" xr3:uid="{FD05CA8E-2FF6-4482-A667-AF6A65E699F6}" name="Font Bold"/>
     <tableColumn id="6" xr3:uid="{FDC8A75C-3349-4AAA-AF78-CD0E21F747FC}" name="Font Color"/>
     <tableColumn id="7" xr3:uid="{61C0565E-B0AB-4FA1-B80E-D0BA900ECEF2}" name="Font Name"/>
+    <tableColumn id="15" xr3:uid="{C9BF7A95-FC3C-42C9-8728-16FDF3E88E6B}" name="Border Color"/>
     <tableColumn id="8" xr3:uid="{137F01B8-CF74-4619-95FF-80537C14834D}" name="Header Background Color"/>
     <tableColumn id="9" xr3:uid="{6E25A935-B2DA-4803-BCE0-5704FE01B154}" name="Header Font Color"/>
     <tableColumn id="10" xr3:uid="{5BE2E524-EFC9-4F41-BE41-FBFB34D249E5}" name="Header Font Size"/>
@@ -604,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A443A47E-CD8A-44BA-8C86-60756BA41290}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -837,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C007B5-97FC-4202-9E75-B2839591FD10}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -851,17 +858,17 @@
     <col min="4" max="4" width="9.921875" customWidth="1"/>
     <col min="5" max="5" width="10.15234375" customWidth="1"/>
     <col min="6" max="6" width="10.921875" customWidth="1"/>
-    <col min="7" max="7" width="11.4609375" customWidth="1"/>
-    <col min="8" max="8" width="23.15234375" customWidth="1"/>
-    <col min="9" max="9" width="17.23046875" customWidth="1"/>
-    <col min="10" max="10" width="16.23046875" customWidth="1"/>
-    <col min="11" max="11" width="16.4609375" customWidth="1"/>
-    <col min="12" max="12" width="17.765625" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.4609375" customWidth="1"/>
+    <col min="9" max="9" width="23.15234375" customWidth="1"/>
+    <col min="10" max="10" width="17.23046875" customWidth="1"/>
+    <col min="11" max="11" width="16.23046875" customWidth="1"/>
+    <col min="12" max="12" width="16.4609375" customWidth="1"/>
+    <col min="13" max="13" width="17.765625" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -884,28 +891,31 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -928,24 +938,27 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>31</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Totals to metadata
</commit_message>
<xml_diff>
--- a/Formatter Metadata.xlsx
+++ b/Formatter Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbe\git\ExcelFormatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE51006-7A47-43D6-A1E4-DE3B4450DEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA9D146-478C-403D-BBBE-839E6315D444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{3832C974-4C9A-4706-B622-9E1F931418CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="50">
   <si>
     <t>Field Name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>XLSX</t>
   </si>
   <si>
-    <t>Employee Survey PDF</t>
-  </si>
-  <si>
     <t>PDF</t>
   </si>
   <si>
@@ -181,6 +178,15 @@
   </si>
   <si>
     <t>Page</t>
+  </si>
+  <si>
+    <t>ESPDF</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Heading Totals</t>
   </si>
 </sst>
 </file>
@@ -270,9 +276,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0">
-  <autoFilter ref="A1:K8" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}" name="Table1" displayName="Table1" ref="A1:L15" totalsRowShown="0">
+  <autoFilter ref="A1:L15" xr:uid="{6D93055F-DD49-405D-8ADB-D622B314AAC3}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{536BAD92-DDD9-4494-936F-87D0426E704B}" name="Report Name"/>
     <tableColumn id="2" xr3:uid="{6A91D369-F2C3-4116-8219-E95FB21560C7}" name="Field Name" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{E70DEC8B-06B4-4D01-BFA5-944FFB97C62F}" name="Is Header"/>
@@ -284,19 +290,21 @@
     <tableColumn id="9" xr3:uid="{70D5DE6C-14DB-4298-8D02-0C070ABB7466}" name="Font Name"/>
     <tableColumn id="11" xr3:uid="{41856FA6-3460-4871-88F9-7A854FBFECD8}" name="Wrap Text"/>
     <tableColumn id="10" xr3:uid="{3B76F452-F0AE-4EEE-8206-08977C35E851}" name="Number Format"/>
+    <tableColumn id="12" xr3:uid="{CED23F33-8BC7-48E6-A1B6-EC4D0106F864}" name="Totals"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}" name="Table2" displayName="Table2" ref="A1:Q3" totalsRowShown="0">
-  <autoFilter ref="A1:Q3" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}" name="Table2" displayName="Table2" ref="A1:R3" totalsRowShown="0">
+  <autoFilter ref="A1:R3" xr:uid="{AA701D72-4CCC-492B-9ACD-E2A5FA795BEF}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{819CCBB3-CE38-46C5-BF73-9CAC9404EA8B}" name="Report Name"/>
     <tableColumn id="2" xr3:uid="{05D5A490-4E2E-476F-BC4B-0E02930681C1}" name="CSV File"/>
     <tableColumn id="3" xr3:uid="{4ABA2077-D15A-4C80-80AE-C8CA6FF82335}" name="Title"/>
     <tableColumn id="17" xr3:uid="{759F6AA9-2BC8-4D5D-8439-ED90FD8677A2}" name="Heading Type"/>
+    <tableColumn id="18" xr3:uid="{AF618F92-2C74-4E66-AAB9-316614C2DAE4}" name="Heading Totals"/>
     <tableColumn id="4" xr3:uid="{032540CA-C8B4-4401-8337-0BA2943F47FD}" name="Font Size"/>
     <tableColumn id="5" xr3:uid="{FD05CA8E-2FF6-4482-A667-AF6A65E699F6}" name="Font Bold"/>
     <tableColumn id="6" xr3:uid="{FDC8A75C-3349-4AAA-AF78-CD0E21F747FC}" name="Font Color"/>
@@ -632,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A443A47E-CD8A-44BA-8C86-60756BA41290}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -652,7 +660,7 @@
     <col min="11" max="11" width="15.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -686,8 +694,11 @@
       <c r="K1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -713,7 +724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -736,7 +747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -762,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -785,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -808,7 +819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -831,7 +842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -855,6 +866,179 @@
       </c>
       <c r="K8" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -867,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C007B5-97FC-4202-9E75-B2839591FD10}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -878,22 +1062,22 @@
     <col min="1" max="1" width="18.23046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.07421875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53515625" customWidth="1"/>
-    <col min="5" max="5" width="9.921875" customWidth="1"/>
-    <col min="6" max="6" width="10.15234375" customWidth="1"/>
-    <col min="7" max="7" width="10.921875" customWidth="1"/>
-    <col min="8" max="9" width="11.4609375" customWidth="1"/>
-    <col min="10" max="10" width="23.15234375" customWidth="1"/>
-    <col min="11" max="11" width="17.23046875" customWidth="1"/>
-    <col min="12" max="12" width="16.23046875" customWidth="1"/>
-    <col min="13" max="13" width="16.4609375" customWidth="1"/>
-    <col min="14" max="14" width="17.765625" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.53515625" customWidth="1"/>
+    <col min="6" max="6" width="9.921875" customWidth="1"/>
+    <col min="7" max="7" width="10.15234375" customWidth="1"/>
+    <col min="8" max="8" width="10.921875" customWidth="1"/>
+    <col min="9" max="10" width="11.4609375" customWidth="1"/>
+    <col min="11" max="11" width="23.15234375" customWidth="1"/>
+    <col min="12" max="12" width="17.23046875" customWidth="1"/>
+    <col min="13" max="13" width="16.23046875" customWidth="1"/>
+    <col min="14" max="14" width="16.4609375" customWidth="1"/>
+    <col min="15" max="15" width="17.765625" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -904,49 +1088,52 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -957,51 +1144,54 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
       <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
         <v>36</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1010,46 +1200,49 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
       <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
       <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
       <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="Q3" t="s">
-        <v>44</v>
+      <c r="R3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>